<commit_message>
updated TC08, TC10, TC11
</commit_message>
<xml_diff>
--- a/target/test-classes/TestData/NewData.xlsx
+++ b/target/test-classes/TestData/NewData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jteja\GFLAutomation\GFL.Wishes\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9E6A2D-0BA3-4790-BD93-94C9A37994F1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631D04B3-4CE9-49F0-9464-8A06C3FCB838}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="15" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{24025A28-F3F9-43F5-89B1-20F9E5BBA4E0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{24025A28-F3F9-43F5-89B1-20F9E5BBA4E0}"/>
   </bookViews>
   <sheets>
     <sheet name="RunModes" sheetId="1" r:id="rId1"/>

</xml_diff>